<commit_message>
Fix Enhancement job detection with CSV fallback
- Added CSV import mode when Jobber API job type detection fails
- Added flexible date parsing for multiple date formats
- Properly filters by Job Type column for Enhancement/Contracted Enhancement
- January 2026 report now shows 30 enhancement jobs ($35,405.75 revenue)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/1-OneOffReport-January.xlsx
+++ b/1-OneOffReport-January.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Executive Dashboard" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Jobs" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Invoices" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Executive Dashboard" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jobs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Invoices" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,8 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_($* #,##0_);_($* (#,##0);_($* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_($* #,##0.00_);_($* (#,##0.00);_($* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -65,7 +66,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -82,6 +83,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="001B365D"/>
         <bgColor rgb="001B365D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8F9FA"/>
+        <bgColor rgb="00F8F9FA"/>
       </patternFill>
     </fill>
   </fills>
@@ -111,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -122,10 +129,32 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00C6EFCE"/>
+          <bgColor rgb="00C6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFC7CE"/>
+          <bgColor rgb="00FFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -515,7 +544,7 @@
     <row r="3">
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Generated: February 02, 2026 at 01:36 AM</t>
+          <t>Generated: February 01, 2026 at 08:50 PM</t>
         </is>
       </c>
     </row>
@@ -541,22 +570,22 @@
     </row>
     <row r="7">
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="n"/>
       <c r="D7" s="6" t="n">
-        <v>0</v>
+        <v>35405.75</v>
       </c>
       <c r="E7" s="4" t="n"/>
       <c r="F7" s="6" t="n">
-        <v>0</v>
+        <v>13409.02</v>
       </c>
       <c r="G7" s="4" t="n"/>
     </row>
     <row r="8">
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>0 std / 0 contracted</t>
+          <t>29 std / 1 contracted</t>
         </is>
       </c>
       <c r="C8" s="4" t="n"/>
@@ -564,7 +593,7 @@
       <c r="E8" s="4" t="n"/>
       <c r="F8" s="8" t="inlineStr">
         <is>
-          <t>margin: 0.0%</t>
+          <t>margin: 37.9%</t>
         </is>
       </c>
       <c r="G8" s="4" t="n"/>
@@ -584,7 +613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -594,14 +623,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="7" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="6" customWidth="1" min="7" max="7"/>
-    <col width="8" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="8" max="8"/>
+    <col width="24" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -651,7 +680,1245 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="10" t="inlineStr">
+        <is>
+          <t>11652</t>
+        </is>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C2" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F2" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G2" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I2" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>11651</t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C3" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E3" s="12" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F3" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G3" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I3" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>11650</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C4" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F4" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I4" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
+          <t>11649</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C5" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D5" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E5" s="12" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F5" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G5" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I5" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>11648</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C6" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I6" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t>11647</t>
+        </is>
+      </c>
+      <c r="B7" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C7" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D7" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E7" s="12" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F7" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I7" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>11646</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C8" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I8" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="12" t="inlineStr">
+        <is>
+          <t>11645</t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C9" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D9" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E9" s="12" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F9" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G9" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I9" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>11644</t>
+        </is>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C10" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I10" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="12" t="inlineStr">
+        <is>
+          <t>11643</t>
+        </is>
+      </c>
+      <c r="B11" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C11" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D11" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E11" s="12" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F11" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G11" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I11" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>11642</t>
+        </is>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F12" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I12" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t>11641</t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C13" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D13" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E13" s="12" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F13" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G13" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I13" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="inlineStr">
+        <is>
+          <t>11640</t>
+        </is>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F14" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I14" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="12" t="inlineStr">
+        <is>
+          <t>11639</t>
+        </is>
+      </c>
+      <c r="B15" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C15" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D15" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E15" s="12" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F15" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G15" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I15" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>11638</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F16" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G16" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I16" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="12" t="inlineStr">
+        <is>
+          <t>11637</t>
+        </is>
+      </c>
+      <c r="B17" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C17" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D17" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E17" s="12" t="inlineStr">
+        <is>
+          <t>Jan 31, 20</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="G17" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="13" t="n">
+        <v>895.9299999999999</v>
+      </c>
+      <c r="I17" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
+        <is>
+          <t>11578</t>
+        </is>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>Inter Atlanta FC</t>
+        </is>
+      </c>
+      <c r="C18" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D18" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E18" s="10" t="inlineStr">
+        <is>
+          <t>Jan 27, 20</t>
+        </is>
+      </c>
+      <c r="F18" s="11" t="n">
+        <v>482</v>
+      </c>
+      <c r="G18" s="11" t="n">
+        <v>526.0700000000001</v>
+      </c>
+      <c r="H18" s="11" t="n">
+        <v>-44.07000000000005</v>
+      </c>
+      <c r="I18" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="12" t="inlineStr">
+        <is>
+          <t>11577</t>
+        </is>
+      </c>
+      <c r="B19" s="12" t="inlineStr">
+        <is>
+          <t>Inter Atlanta FC</t>
+        </is>
+      </c>
+      <c r="C19" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D19" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E19" s="12" t="inlineStr">
+        <is>
+          <t>Jan 26, 20</t>
+        </is>
+      </c>
+      <c r="F19" s="13" t="n">
+        <v>2496</v>
+      </c>
+      <c r="G19" s="13" t="n">
+        <v>3087.62</v>
+      </c>
+      <c r="H19" s="13" t="n">
+        <v>-591.6199999999999</v>
+      </c>
+      <c r="I19" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="inlineStr">
+        <is>
+          <t>11556</t>
+        </is>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>Inter Atlanta FC</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E20" s="10" t="inlineStr">
+        <is>
+          <t>Jan 19, 20</t>
+        </is>
+      </c>
+      <c r="F20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12" t="inlineStr">
+        <is>
+          <t>11528</t>
+        </is>
+      </c>
+      <c r="B21" s="12" t="inlineStr">
+        <is>
+          <t>Kim King Associates</t>
+        </is>
+      </c>
+      <c r="C21" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D21" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E21" s="12" t="inlineStr">
+        <is>
+          <t>Jan 16, 20</t>
+        </is>
+      </c>
+      <c r="F21" s="13" t="n">
+        <v>1917.5</v>
+      </c>
+      <c r="G21" s="13" t="n">
+        <v>1475</v>
+      </c>
+      <c r="H21" s="13" t="n">
+        <v>442.5</v>
+      </c>
+      <c r="I21" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>11521</t>
+        </is>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>Mary Smith</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D22" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E22" s="10" t="inlineStr">
+        <is>
+          <t>Jan 15, 20</t>
+        </is>
+      </c>
+      <c r="F22" s="11" t="n">
+        <v>450</v>
+      </c>
+      <c r="G22" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11" t="n">
+        <v>450</v>
+      </c>
+      <c r="I22" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="12" t="inlineStr">
+        <is>
+          <t>11520</t>
+        </is>
+      </c>
+      <c r="B23" s="12" t="inlineStr">
+        <is>
+          <t>Reagan Burford</t>
+        </is>
+      </c>
+      <c r="C23" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D23" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E23" s="12" t="inlineStr">
+        <is>
+          <t>Jan 13, 20</t>
+        </is>
+      </c>
+      <c r="F23" s="13" t="n">
+        <v>175</v>
+      </c>
+      <c r="G23" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13" t="n">
+        <v>175</v>
+      </c>
+      <c r="I23" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="inlineStr">
+        <is>
+          <t>11474</t>
+        </is>
+      </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>Kim King Associates</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>Contracted Enhancement</t>
+        </is>
+      </c>
+      <c r="D24" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E24" s="10" t="inlineStr">
+        <is>
+          <t>Jan 08, 20</t>
+        </is>
+      </c>
+      <c r="F24" s="11" t="n">
+        <v>2640</v>
+      </c>
+      <c r="G24" s="11" t="n">
+        <v>2200</v>
+      </c>
+      <c r="H24" s="11" t="n">
+        <v>440</v>
+      </c>
+      <c r="I24" s="10" t="inlineStr">
+        <is>
+          <t>Contracted Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="12" t="inlineStr">
+        <is>
+          <t>11473</t>
+        </is>
+      </c>
+      <c r="B25" s="12" t="inlineStr">
+        <is>
+          <t>Inter Atlanta FC</t>
+        </is>
+      </c>
+      <c r="C25" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D25" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E25" s="12" t="inlineStr">
+        <is>
+          <t>Jan 13, 20</t>
+        </is>
+      </c>
+      <c r="F25" s="13" t="n">
+        <v>4050</v>
+      </c>
+      <c r="G25" s="13" t="n">
+        <v>10239.93</v>
+      </c>
+      <c r="H25" s="13" t="n">
+        <v>-6189.93</v>
+      </c>
+      <c r="I25" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="inlineStr">
+        <is>
+          <t>11416</t>
+        </is>
+      </c>
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>Max Slater</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D26" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E26" s="10" t="inlineStr">
+        <is>
+          <t>Jan 07, 20</t>
+        </is>
+      </c>
+      <c r="F26" s="11" t="n">
+        <v>992</v>
+      </c>
+      <c r="G26" s="11" t="n">
+        <v>445.25</v>
+      </c>
+      <c r="H26" s="11" t="n">
+        <v>546.75</v>
+      </c>
+      <c r="I26" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="12" t="inlineStr">
+        <is>
+          <t>11415</t>
+        </is>
+      </c>
+      <c r="B27" s="12" t="inlineStr">
+        <is>
+          <t>Max Slater</t>
+        </is>
+      </c>
+      <c r="C27" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D27" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E27" s="12" t="inlineStr">
+        <is>
+          <t>Jan 12, 20</t>
+        </is>
+      </c>
+      <c r="F27" s="13" t="n">
+        <v>951.13</v>
+      </c>
+      <c r="G27" s="13" t="n">
+        <v>1003.06</v>
+      </c>
+      <c r="H27" s="13" t="n">
+        <v>-51.92999999999995</v>
+      </c>
+      <c r="I27" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="inlineStr">
+        <is>
+          <t>11407</t>
+        </is>
+      </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>Greg Reihing</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D28" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E28" s="10" t="inlineStr">
+        <is>
+          <t>Jan 12, 20</t>
+        </is>
+      </c>
+      <c r="F28" s="11" t="n">
+        <v>549.25</v>
+      </c>
+      <c r="G28" s="11" t="n">
+        <v>652.42</v>
+      </c>
+      <c r="H28" s="11" t="n">
+        <v>-103.17</v>
+      </c>
+      <c r="I28" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="12" t="inlineStr">
+        <is>
+          <t>11314</t>
+        </is>
+      </c>
+      <c r="B29" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C29" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D29" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E29" s="12" t="inlineStr">
+        <is>
+          <t>Jan 06, 20</t>
+        </is>
+      </c>
+      <c r="F29" s="13" t="n">
+        <v>3887.99</v>
+      </c>
+      <c r="G29" s="13" t="n">
+        <v>1553.32</v>
+      </c>
+      <c r="H29" s="13" t="n">
+        <v>2334.67</v>
+      </c>
+      <c r="I29" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10" t="inlineStr">
+        <is>
+          <t>11303</t>
+        </is>
+      </c>
+      <c r="B30" s="10" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C30" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D30" s="10" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E30" s="10" t="inlineStr">
+        <is>
+          <t>Jan 05, 20</t>
+        </is>
+      </c>
+      <c r="F30" s="11" t="n">
+        <v>1240</v>
+      </c>
+      <c r="G30" s="11" t="n">
+        <v>407.03</v>
+      </c>
+      <c r="H30" s="11" t="n">
+        <v>832.97</v>
+      </c>
+      <c r="I30" s="10" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="12" t="inlineStr">
+        <is>
+          <t>11302</t>
+        </is>
+      </c>
+      <c r="B31" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C31" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D31" s="12" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="E31" s="12" t="inlineStr">
+        <is>
+          <t>Jan 05, 20</t>
+        </is>
+      </c>
+      <c r="F31" s="13" t="n">
+        <v>1240</v>
+      </c>
+      <c r="G31" s="13" t="n">
+        <v>407.03</v>
+      </c>
+      <c r="H31" s="13" t="n">
+        <v>832.97</v>
+      </c>
+      <c r="I31" s="12" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="H2:H31">
+    <cfRule type="expression" priority="1" dxfId="0">
+      <formula>$H2&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" priority="2" dxfId="1">
+      <formula>$H2&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -662,7 +1929,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -708,6 +1975,461 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="12" t="inlineStr">
+        <is>
+          <t>17096</t>
+        </is>
+      </c>
+      <c r="B2" s="12" t="inlineStr">
+        <is>
+          <t>Inter Atlanta FC</t>
+        </is>
+      </c>
+      <c r="C2" s="12" t="inlineStr">
+        <is>
+          <t>11578</t>
+        </is>
+      </c>
+      <c r="D2" s="13" t="n">
+        <v>482</v>
+      </c>
+      <c r="E2" s="12" t="inlineStr">
+        <is>
+          <t>Awaiting Payment</t>
+        </is>
+      </c>
+      <c r="F2" s="12" t="inlineStr">
+        <is>
+          <t>Jan 30, 2026</t>
+        </is>
+      </c>
+      <c r="G2" s="12" t="inlineStr">
+        <is>
+          <t>Feb 14, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>17095</t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t>Inter Atlanta FC</t>
+        </is>
+      </c>
+      <c r="C3" s="12" t="inlineStr">
+        <is>
+          <t>11577</t>
+        </is>
+      </c>
+      <c r="D3" s="13" t="n">
+        <v>2496</v>
+      </c>
+      <c r="E3" s="12" t="inlineStr">
+        <is>
+          <t>Awaiting Payment</t>
+        </is>
+      </c>
+      <c r="F3" s="12" t="inlineStr">
+        <is>
+          <t>Jan 30, 2026</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="inlineStr">
+        <is>
+          <t>Feb 14, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>17094</t>
+        </is>
+      </c>
+      <c r="B4" s="12" t="inlineStr">
+        <is>
+          <t>Mary Smith</t>
+        </is>
+      </c>
+      <c r="C4" s="12" t="inlineStr">
+        <is>
+          <t>11521</t>
+        </is>
+      </c>
+      <c r="D4" s="13" t="n">
+        <v>450</v>
+      </c>
+      <c r="E4" s="12" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F4" s="12" t="inlineStr">
+        <is>
+          <t>Jan 22, 2026</t>
+        </is>
+      </c>
+      <c r="G4" s="12" t="inlineStr">
+        <is>
+          <t>Jan 22, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
+          <t>17093</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>Kim King Associates</t>
+        </is>
+      </c>
+      <c r="C5" s="12" t="inlineStr">
+        <is>
+          <t>11528</t>
+        </is>
+      </c>
+      <c r="D5" s="13" t="n">
+        <v>1917.5</v>
+      </c>
+      <c r="E5" s="12" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>Jan 19, 2026</t>
+        </is>
+      </c>
+      <c r="G5" s="12" t="inlineStr">
+        <is>
+          <t>Feb 03, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>17092</t>
+        </is>
+      </c>
+      <c r="B6" s="12" t="inlineStr">
+        <is>
+          <t>Inter Atlanta FC</t>
+        </is>
+      </c>
+      <c r="C6" s="12" t="inlineStr">
+        <is>
+          <t>11473</t>
+        </is>
+      </c>
+      <c r="D6" s="13" t="n">
+        <v>4050</v>
+      </c>
+      <c r="E6" s="12" t="inlineStr">
+        <is>
+          <t>Awaiting Payment</t>
+        </is>
+      </c>
+      <c r="F6" s="12" t="inlineStr">
+        <is>
+          <t>Jan 22, 2026</t>
+        </is>
+      </c>
+      <c r="G6" s="12" t="inlineStr">
+        <is>
+          <t>Feb 06, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t>17091</t>
+        </is>
+      </c>
+      <c r="B7" s="12" t="inlineStr">
+        <is>
+          <t>Max Slater</t>
+        </is>
+      </c>
+      <c r="C7" s="12" t="inlineStr">
+        <is>
+          <t>11415</t>
+        </is>
+      </c>
+      <c r="D7" s="13" t="n">
+        <v>951.13</v>
+      </c>
+      <c r="E7" s="12" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F7" s="12" t="inlineStr">
+        <is>
+          <t>Jan 14, 2026</t>
+        </is>
+      </c>
+      <c r="G7" s="12" t="inlineStr">
+        <is>
+          <t>Jan 14, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="12" t="inlineStr">
+        <is>
+          <t>17090</t>
+        </is>
+      </c>
+      <c r="B8" s="12" t="inlineStr">
+        <is>
+          <t>Greg Reihing</t>
+        </is>
+      </c>
+      <c r="C8" s="12" t="inlineStr">
+        <is>
+          <t>11407</t>
+        </is>
+      </c>
+      <c r="D8" s="13" t="n">
+        <v>549.25</v>
+      </c>
+      <c r="E8" s="12" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F8" s="12" t="inlineStr">
+        <is>
+          <t>Jan 14, 2026</t>
+        </is>
+      </c>
+      <c r="G8" s="12" t="inlineStr">
+        <is>
+          <t>Jan 14, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="12" t="inlineStr">
+        <is>
+          <t>17089</t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="inlineStr">
+        <is>
+          <t>Reagan Burford</t>
+        </is>
+      </c>
+      <c r="C9" s="12" t="inlineStr">
+        <is>
+          <t>11520</t>
+        </is>
+      </c>
+      <c r="D9" s="13" t="n">
+        <v>175</v>
+      </c>
+      <c r="E9" s="12" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F9" s="12" t="inlineStr">
+        <is>
+          <t>Jan 13, 2026</t>
+        </is>
+      </c>
+      <c r="G9" s="12" t="inlineStr">
+        <is>
+          <t>Jan 13, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="12" t="inlineStr">
+        <is>
+          <t>17088</t>
+        </is>
+      </c>
+      <c r="B10" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C10" s="12" t="inlineStr">
+        <is>
+          <t>11314</t>
+        </is>
+      </c>
+      <c r="D10" s="13" t="n">
+        <v>3887.99</v>
+      </c>
+      <c r="E10" s="12" t="inlineStr">
+        <is>
+          <t>Awaiting Payment</t>
+        </is>
+      </c>
+      <c r="F10" s="12" t="inlineStr">
+        <is>
+          <t>Jan 12, 2026</t>
+        </is>
+      </c>
+      <c r="G10" s="12" t="inlineStr">
+        <is>
+          <t>Feb 11, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="12" t="inlineStr">
+        <is>
+          <t>17087</t>
+        </is>
+      </c>
+      <c r="B11" s="12" t="inlineStr">
+        <is>
+          <t>Kim King Associates</t>
+        </is>
+      </c>
+      <c r="C11" s="12" t="inlineStr">
+        <is>
+          <t>11474</t>
+        </is>
+      </c>
+      <c r="D11" s="13" t="n">
+        <v>2640</v>
+      </c>
+      <c r="E11" s="12" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Jan 12, 2026</t>
+        </is>
+      </c>
+      <c r="G11" s="12" t="inlineStr">
+        <is>
+          <t>Jan 27, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="12" t="inlineStr">
+        <is>
+          <t>17086</t>
+        </is>
+      </c>
+      <c r="B12" s="12" t="inlineStr">
+        <is>
+          <t>Max Slater</t>
+        </is>
+      </c>
+      <c r="C12" s="12" t="inlineStr">
+        <is>
+          <t>11416</t>
+        </is>
+      </c>
+      <c r="D12" s="13" t="n">
+        <v>992</v>
+      </c>
+      <c r="E12" s="12" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F12" s="12" t="inlineStr">
+        <is>
+          <t>Jan 12, 2026</t>
+        </is>
+      </c>
+      <c r="G12" s="12" t="inlineStr">
+        <is>
+          <t>Jan 12, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t>17081</t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C13" s="12" t="inlineStr">
+        <is>
+          <t>11302</t>
+        </is>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>1240</v>
+      </c>
+      <c r="E13" s="12" t="inlineStr">
+        <is>
+          <t>Awaiting Payment</t>
+        </is>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>Jan 07, 2026</t>
+        </is>
+      </c>
+      <c r="G13" s="12" t="inlineStr">
+        <is>
+          <t>Feb 06, 2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="12" t="inlineStr">
+        <is>
+          <t>17080</t>
+        </is>
+      </c>
+      <c r="B14" s="12" t="inlineStr">
+        <is>
+          <t>Comcast Corporation</t>
+        </is>
+      </c>
+      <c r="C14" s="12" t="inlineStr">
+        <is>
+          <t>11303</t>
+        </is>
+      </c>
+      <c r="D14" s="13" t="n">
+        <v>1240</v>
+      </c>
+      <c r="E14" s="12" t="inlineStr">
+        <is>
+          <t>Awaiting Payment</t>
+        </is>
+      </c>
+      <c r="F14" s="12" t="inlineStr">
+        <is>
+          <t>Jan 07, 2026</t>
+        </is>
+      </c>
+      <c r="G14" s="12" t="inlineStr">
+        <is>
+          <t>Feb 06, 2026</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>